<commit_message>
Selenium Final Exam - Boris
Added 10 additional test cases
</commit_message>
<xml_diff>
--- a/manualTestCases/Luma_Test_Casess.xlsx
+++ b/manualTestCases/Luma_Test_Casess.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borisabunagimov/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fiverr-QA\Lake_J\Laike\NewClone\Final_exam_Selenium\manualTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5764A7F1-B652-2A41-8DD0-046D91EAEE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="135">
   <si>
     <t>TC - ID</t>
   </si>
@@ -82,9 +81,6 @@
   </si>
   <si>
     <t>Test 012</t>
-  </si>
-  <si>
-    <t>TTest 013</t>
   </si>
   <si>
     <t>Test 014</t>
@@ -410,11 +406,200 @@
   <si>
     <t>1.Account information should be visible</t>
   </si>
+  <si>
+    <t>Verify that user can't  create a new account without First Name</t>
+  </si>
+  <si>
+    <t>1. visit: https://magento.softwaretestingboard.com/ 
+2. Click on create an account button
+3. Under personal information fill Last Name
+4. under sugnin information fill Email, password and Confirm password
+5. Click create an account button</t>
+  </si>
+  <si>
+    <t>1. User should now create new user
+2. First Name field error should appear</t>
+  </si>
+  <si>
+    <t>Verify that user can't  create a new account without Last Name</t>
+  </si>
+  <si>
+    <t>1. visit: https://magento.softwaretestingboard.com/ 
+2. Click on create an account button
+3. Under personal information fill First Name
+4. under sugnin information fill Email, password and Confirm password
+5. Click create an account button</t>
+  </si>
+  <si>
+    <t>1. visit: https://magento.softwaretestingboard.com/ 
+2. Click on create an account button
+3. Under personal information fill First Name and Last Name
+4. under sugnin information, fill password and Confirm password
+5. Click create an account button</t>
+  </si>
+  <si>
+    <t>1. User should now create new user
+2. Last Name field error should appear</t>
+  </si>
+  <si>
+    <t>1. User should now create new user
+2. Email Name field error should appear</t>
+  </si>
+  <si>
+    <t>Verify that user can't  create a new account without Email Name</t>
+  </si>
+  <si>
+    <t>Verify that user can't  create a new account without Password Name</t>
+  </si>
+  <si>
+    <t>1. visit: https://magento.softwaretestingboard.com/ 
+2. Click on create an account button
+3. Under personal information fill First Name and Last Name
+4. under sugnin information, fill Email
+5. Click create an account button</t>
+  </si>
+  <si>
+    <t>1. User should now create new user
+2. Password Name field error should appear</t>
+  </si>
+  <si>
+    <t>Test 013</t>
+  </si>
+  <si>
+    <t>Test 021</t>
+  </si>
+  <si>
+    <t>Test 022</t>
+  </si>
+  <si>
+    <t>Test 023</t>
+  </si>
+  <si>
+    <t>Test 024</t>
+  </si>
+  <si>
+    <t>Test 025</t>
+  </si>
+  <si>
+    <t>Verify that user can't login with wrong credentials</t>
+  </si>
+  <si>
+    <t>1. visit: https://magento.softwaretestingboard.com/
+2. Click on sign in button
+3. Type wrong email and password in login form
+4. click on signin button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.user should not login 
+2. user should see validation erros </t>
+  </si>
+  <si>
+    <t>Verify that user can't login with empty  credentials</t>
+  </si>
+  <si>
+    <t>1. visit: https://magento.softwaretestingboard.com/
+2. Click on sign in button
+3. leave email and password field empty 
+4. click on signin button.</t>
+  </si>
+  <si>
+    <t>Test 026</t>
+  </si>
+  <si>
+    <t>Test 027</t>
+  </si>
+  <si>
+    <t>Verify that user can sort product with Name</t>
+  </si>
+  <si>
+    <t>"1. click on search field
+2. input any product name
+4 Related product should be displayed
+5. Click on sort filter on right side and select ""product name"" from drop down</t>
+  </si>
+  <si>
+    <t>1.Product should be sorted by product name in ascending or descending order</t>
+  </si>
+  <si>
+    <t>Verify that user can sort product with Price</t>
+  </si>
+  <si>
+    <t>"1. click on search field
+2. input any product name
+4 Related product should be displayed
+5. Click on sort filter on right side and select ""price"" from drop down</t>
+  </si>
+  <si>
+    <t>1.Product should be sorted by product price in ascending or descending order</t>
+  </si>
+  <si>
+    <t>Test 028</t>
+  </si>
+  <si>
+    <t>Test 029</t>
+  </si>
+  <si>
+    <t>Verify that user can sort product by Relevance</t>
+  </si>
+  <si>
+    <t>"1. click on search field
+2. input any product name
+4 Related product should be displayed
+5. Click on sort filter on right side and select ""Relevance"" from drop down</t>
+  </si>
+  <si>
+    <t>1.Product should be sorted by product relevance in ascending or descending order</t>
+  </si>
+  <si>
+    <t>Show 12 products per page</t>
+  </si>
+  <si>
+    <t>"1. click on search field
+2. input any product name
+4 Related product should be displayed
+5. scroll to end of the page and select 12 from dropdown</t>
+  </si>
+  <si>
+    <t>1. 12 products should display on the page</t>
+  </si>
+  <si>
+    <t>Show 24 products per page</t>
+  </si>
+  <si>
+    <t>"1. click on search field
+2. input any product name
+4 Related product should be displayed
+5. scroll to end of the page and select 24 from dropdown</t>
+  </si>
+  <si>
+    <t>1. 24 products should display on the page</t>
+  </si>
+  <si>
+    <t>Show 36 products per page</t>
+  </si>
+  <si>
+    <t>"1. click on search field
+2. input any product name
+4 Related product should be displayed
+5. scroll to end of the page and select 36 from dropdown</t>
+  </si>
+  <si>
+    <t>1. 36 products should display on the page</t>
+  </si>
+  <si>
+    <t>Test 030</t>
+  </si>
+  <si>
+    <t>Test 031</t>
+  </si>
+  <si>
+    <t>Test 032</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -603,7 +788,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -613,6 +797,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -894,28 +1084,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="147.5" customWidth="1"/>
-    <col min="5" max="5" width="0.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="59.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.5" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="147.42578125" customWidth="1"/>
+    <col min="5" max="5" width="0.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="59.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -939,20 +1129,20 @@
       </c>
       <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="73.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
@@ -962,7 +1152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -973,19 +1163,19 @@
       <c r="I3" s="1"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>31</v>
+      <c r="C4" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="13" t="s">
-        <v>32</v>
+      <c r="F4" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
@@ -995,30 +1185,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="8"/>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>34</v>
+    <row r="6" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>91</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="15" t="s">
-        <v>35</v>
+      <c r="F6" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
@@ -1028,30 +1218,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>37</v>
+      <c r="C8" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="12" t="s">
-        <v>38</v>
+      <c r="F8" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
@@ -1061,30 +1251,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>40</v>
+      <c r="C10" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="15" t="s">
-        <v>41</v>
+      <c r="F10" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
@@ -1094,30 +1284,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+    <row r="12" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="18" t="s">
-        <v>73</v>
+      <c r="F12" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7" t="s">
@@ -1127,30 +1317,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+    <row r="14" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="19" t="s">
-        <v>74</v>
+      <c r="F14" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7" t="s">
@@ -1160,30 +1350,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+    <row r="16" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="12" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7" t="s">
@@ -1193,7 +1383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="8"/>
@@ -1204,19 +1394,19 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+    <row r="18" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="19" t="s">
-        <v>76</v>
+      <c r="F18" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7" t="s">
@@ -1226,7 +1416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="8"/>
@@ -1237,19 +1427,19 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+    <row r="20" spans="2:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="18" t="s">
-        <v>77</v>
+      <c r="F20" s="17" t="s">
+        <v>72</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7" t="s">
@@ -1259,7 +1449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="8"/>
@@ -1270,19 +1460,19 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
+    <row r="22" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>53</v>
+        <v>43</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="15" t="s">
-        <v>78</v>
+      <c r="F22" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7" t="s">
@@ -1292,30 +1482,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
+    <row r="24" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="18" t="s">
-        <v>79</v>
+      <c r="F24" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7" t="s">
@@ -1325,30 +1515,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="6"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
-        <v>19</v>
+    <row r="26" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="15" t="s">
+        <v>99</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="E26" s="7"/>
-      <c r="F26" s="19" t="s">
-        <v>80</v>
+      <c r="F26" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7" t="s">
@@ -1358,30 +1548,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
       <c r="G27" s="8"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
-        <v>20</v>
+    <row r="28" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E28" s="7"/>
-      <c r="F28" s="12" t="s">
-        <v>81</v>
+      <c r="F28" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7" t="s">
@@ -1391,7 +1581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="8"/>
@@ -1402,19 +1592,19 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="2:10" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
-        <v>21</v>
+    <row r="30" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="19" t="s">
-        <v>82</v>
+      <c r="F30" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7" t="s">
@@ -1424,30 +1614,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
-        <v>22</v>
+    <row r="32" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="15" t="s">
+        <v>21</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E32" s="7"/>
-      <c r="F32" s="12" t="s">
-        <v>83</v>
+      <c r="F32" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7" t="s">
@@ -1457,30 +1647,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="6"/>
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="s">
-        <v>23</v>
+    <row r="34" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="E34" s="7"/>
-      <c r="F34" s="15" t="s">
-        <v>84</v>
+      <c r="F34" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7" t="s">
@@ -1490,30 +1680,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="16" t="s">
-        <v>24</v>
+    <row r="36" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="s">
@@ -1523,7 +1713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="8"/>
@@ -1534,19 +1724,19 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="16" t="s">
-        <v>25</v>
+    <row r="38" spans="2:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>69</v>
+        <v>59</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="E38" s="7"/>
-      <c r="F38" s="19" t="s">
-        <v>86</v>
+      <c r="F38" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7" t="s">
@@ -1556,7 +1746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="8"/>
@@ -1567,19 +1757,19 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="16" t="s">
-        <v>26</v>
+    <row r="40" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7" t="s">
@@ -1589,7 +1779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="8"/>
@@ -1600,9 +1790,405 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
+    <row r="42" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="7"/>
+      <c r="F48" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="2:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="F50" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E52" s="7"/>
+      <c r="F52" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="7"/>
+      <c r="F54" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E56" s="7"/>
+      <c r="F56" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E60" s="7"/>
+      <c r="F60" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="2"/>
+    </row>
+    <row r="62" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E62" s="7"/>
+      <c r="F62" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="2"/>
+    </row>
+    <row r="64" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E64" s="7"/>
+      <c r="F64" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{28DDDC7A-DA57-4F4D-954A-3AF19D919B64}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>